<commit_message>
updated relay settings files to include back-of-a-napkin calc of settings
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>VRMSLL</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>CB Initial State [closed=1; open=0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -194,6 +197,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,8 +889,8 @@
       <c r="F2" s="8">
         <v>0.5</v>
       </c>
-      <c r="G2" s="7">
-        <v>600</v>
+      <c r="G2" s="15">
+        <v>1200</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -889,20 +901,20 @@
       <c r="J2" s="7">
         <v>0</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="16">
+        <v>0.60140653040586012</v>
+      </c>
+      <c r="L2" s="7">
+        <v>1</v>
+      </c>
+      <c r="M2" s="7">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7">
         <v>0.8</v>
       </c>
-      <c r="L2" s="7">
-        <v>1</v>
-      </c>
-      <c r="M2" s="7">
-        <v>1</v>
-      </c>
-      <c r="N2" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O2" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P2" s="7">
         <v>20</v>
@@ -910,8 +922,8 @@
       <c r="Q2" s="7">
         <v>1</v>
       </c>
-      <c r="R2" s="7">
-        <v>0.7</v>
+      <c r="R2" s="14">
+        <v>0.60140653040586012</v>
       </c>
       <c r="S2" s="7">
         <v>2</v>
@@ -945,8 +957,8 @@
       <c r="F3" s="8">
         <v>0.5</v>
       </c>
-      <c r="G3" s="7">
-        <v>600</v>
+      <c r="G3" s="15">
+        <v>1200</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -957,20 +969,20 @@
       <c r="J3" s="7">
         <v>0</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="16">
+        <v>2.9124092514083011</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
         <v>0.8</v>
       </c>
-      <c r="L3" s="7">
-        <v>1</v>
-      </c>
-      <c r="M3" s="7">
-        <v>1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O3" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P3" s="7">
         <v>20</v>
@@ -978,8 +990,8 @@
       <c r="Q3" s="7">
         <v>1</v>
       </c>
-      <c r="R3" s="7">
-        <v>0.7</v>
+      <c r="R3" s="14">
+        <v>2.9124092514083011</v>
       </c>
       <c r="S3" s="7">
         <v>2</v>
@@ -1013,8 +1025,8 @@
       <c r="F4" s="8">
         <v>0.5</v>
       </c>
-      <c r="G4" s="7">
-        <v>600</v>
+      <c r="G4" s="15">
+        <v>1200</v>
       </c>
       <c r="H4" s="10">
         <v>1</v>
@@ -1025,20 +1037,20 @@
       <c r="J4" s="7">
         <v>0</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="16">
+        <v>1.3030474825460301</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
         <v>0.8</v>
       </c>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7">
-        <v>1</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O4" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P4" s="7">
         <v>20</v>
@@ -1046,8 +1058,8 @@
       <c r="Q4" s="7">
         <v>1</v>
       </c>
-      <c r="R4" s="7">
-        <v>0.7</v>
+      <c r="R4" s="14">
+        <v>1.3030474825460301</v>
       </c>
       <c r="S4" s="7">
         <v>2</v>
@@ -1081,8 +1093,8 @@
       <c r="F5" s="8">
         <v>0.5</v>
       </c>
-      <c r="G5" s="7">
-        <v>50</v>
+      <c r="G5" s="15">
+        <v>1200</v>
       </c>
       <c r="H5" s="10">
         <v>1</v>
@@ -1093,20 +1105,20 @@
       <c r="J5" s="7">
         <v>0</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="16">
+        <v>0.10023442173431002</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
         <v>0.8</v>
       </c>
-      <c r="L5" s="7">
-        <v>1</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O5" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P5" s="7">
         <v>20</v>
@@ -1114,8 +1126,8 @@
       <c r="Q5" s="7">
         <v>1</v>
       </c>
-      <c r="R5" s="7">
-        <v>0.7</v>
+      <c r="R5" s="14">
+        <v>0.10023442173431002</v>
       </c>
       <c r="S5" s="7">
         <v>2</v>
@@ -1149,8 +1161,8 @@
       <c r="F6" s="8">
         <v>0.5</v>
       </c>
-      <c r="G6" s="7">
-        <v>250</v>
+      <c r="G6" s="15">
+        <v>1200</v>
       </c>
       <c r="H6" s="10">
         <v>1</v>
@@ -1161,20 +1173,20 @@
       <c r="J6" s="7">
         <v>0</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="16">
+        <v>0.50117210867155004</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
         <v>0.8</v>
       </c>
-      <c r="L6" s="7">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O6" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P6" s="7">
         <v>20</v>
@@ -1182,8 +1194,8 @@
       <c r="Q6" s="7">
         <v>1</v>
       </c>
-      <c r="R6" s="7">
-        <v>0.7</v>
+      <c r="R6" s="14">
+        <v>0.50117210867155004</v>
       </c>
       <c r="S6" s="7">
         <v>2</v>
@@ -1217,8 +1229,8 @@
       <c r="F7" s="8">
         <v>0.5</v>
       </c>
-      <c r="G7" s="7">
-        <v>400</v>
+      <c r="G7" s="15">
+        <v>1200</v>
       </c>
       <c r="H7" s="10">
         <v>1</v>
@@ -1229,20 +1241,20 @@
       <c r="J7" s="7">
         <v>0</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="16">
+        <v>0.75175816300732523</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
         <v>0.8</v>
       </c>
-      <c r="L7" s="7">
-        <v>1</v>
-      </c>
-      <c r="M7" s="7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O7" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P7" s="7">
         <v>20</v>
@@ -1250,8 +1262,8 @@
       <c r="Q7" s="7">
         <v>1</v>
       </c>
-      <c r="R7" s="7">
-        <v>0.7</v>
+      <c r="R7" s="14">
+        <v>0.75175816300732523</v>
       </c>
       <c r="S7" s="7">
         <v>2</v>
@@ -1285,8 +1297,8 @@
       <c r="F8" s="8">
         <v>0.5</v>
       </c>
-      <c r="G8" s="7">
-        <v>50</v>
+      <c r="G8" s="15">
+        <v>1200</v>
       </c>
       <c r="H8" s="10">
         <v>1</v>
@@ -1297,20 +1309,20 @@
       <c r="J8" s="7">
         <v>0</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="16">
+        <v>0.10023442173431002</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
         <v>0.8</v>
       </c>
-      <c r="L8" s="7">
-        <v>1</v>
-      </c>
-      <c r="M8" s="7">
-        <v>1</v>
-      </c>
-      <c r="N8" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O8" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P8" s="7">
         <v>20</v>
@@ -1318,8 +1330,8 @@
       <c r="Q8" s="7">
         <v>1</v>
       </c>
-      <c r="R8" s="7">
-        <v>0.7</v>
+      <c r="R8" s="14">
+        <v>0.10023442173431002</v>
       </c>
       <c r="S8" s="7">
         <v>2</v>
@@ -1353,8 +1365,8 @@
       <c r="F9" s="8">
         <v>0.5</v>
       </c>
-      <c r="G9" s="7">
-        <v>600</v>
+      <c r="G9" s="15">
+        <v>1200</v>
       </c>
       <c r="H9" s="11">
         <v>0</v>
@@ -1365,20 +1377,20 @@
       <c r="J9" s="7">
         <v>0</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="16">
+        <v>2.0604166666666663</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7">
         <v>0.8</v>
       </c>
-      <c r="L9" s="7">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O9" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P9" s="7">
         <v>20</v>
@@ -1386,8 +1398,8 @@
       <c r="Q9" s="7">
         <v>1</v>
       </c>
-      <c r="R9" s="7">
-        <v>0.7</v>
+      <c r="R9" s="14">
+        <v>2.0604166666666663</v>
       </c>
       <c r="S9" s="7">
         <v>2</v>
@@ -1421,8 +1433,8 @@
       <c r="F10" s="8">
         <v>0.5</v>
       </c>
-      <c r="G10" s="7">
-        <v>600</v>
+      <c r="G10" s="15">
+        <v>3500</v>
       </c>
       <c r="H10" s="11">
         <v>0</v>
@@ -1433,20 +1445,20 @@
       <c r="J10" s="7">
         <v>0</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="16">
+        <v>1.4128571428571426</v>
+      </c>
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7">
         <v>0.8</v>
       </c>
-      <c r="L10" s="7">
-        <v>1</v>
-      </c>
-      <c r="M10" s="7">
-        <v>1</v>
-      </c>
-      <c r="N10" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O10" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P10" s="7">
         <v>20</v>
@@ -1454,8 +1466,8 @@
       <c r="Q10" s="7">
         <v>1</v>
       </c>
-      <c r="R10" s="7">
-        <v>0.7</v>
+      <c r="R10" s="14">
+        <v>4.1208333333333327</v>
       </c>
       <c r="S10" s="7">
         <v>2</v>
@@ -1489,8 +1501,8 @@
       <c r="F11" s="8">
         <v>0.5</v>
       </c>
-      <c r="G11" s="7">
-        <v>600</v>
+      <c r="G11" s="15">
+        <v>1200</v>
       </c>
       <c r="H11" s="10">
         <v>1</v>
@@ -1501,20 +1513,20 @@
       <c r="J11" s="7">
         <v>0</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="16">
+        <v>1.3300336730129598</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7">
         <v>0.8</v>
       </c>
-      <c r="L11" s="7">
-        <v>1</v>
-      </c>
-      <c r="M11" s="7">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O11" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P11" s="7">
         <v>20</v>
@@ -1522,8 +1534,8 @@
       <c r="Q11" s="7">
         <v>1</v>
       </c>
-      <c r="R11" s="7">
-        <v>0.7</v>
+      <c r="R11" s="14">
+        <v>1.3300336730129598</v>
       </c>
       <c r="S11" s="7">
         <v>2</v>
@@ -1557,8 +1569,8 @@
       <c r="F12" s="8">
         <v>0.5</v>
       </c>
-      <c r="G12" s="7">
-        <v>600</v>
+      <c r="G12" s="15">
+        <v>3500</v>
       </c>
       <c r="H12" s="11">
         <v>0</v>
@@ -1569,20 +1581,20 @@
       <c r="J12" s="7">
         <v>0</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="16">
+        <v>1.4128571428571426</v>
+      </c>
+      <c r="L12" s="7">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1</v>
+      </c>
+      <c r="N12" s="7">
         <v>0.8</v>
       </c>
-      <c r="L12" s="7">
-        <v>1</v>
-      </c>
-      <c r="M12" s="7">
-        <v>1</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O12" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P12" s="7">
         <v>20</v>
@@ -1590,8 +1602,8 @@
       <c r="Q12" s="7">
         <v>1</v>
       </c>
-      <c r="R12" s="7">
-        <v>0.7</v>
+      <c r="R12" s="14">
+        <v>4.1208333333333327</v>
       </c>
       <c r="S12" s="7">
         <v>2</v>
@@ -1625,8 +1637,8 @@
       <c r="F13" s="8">
         <v>0.5</v>
       </c>
-      <c r="G13" s="7">
-        <v>250</v>
+      <c r="G13" s="15">
+        <v>1200</v>
       </c>
       <c r="H13" s="10">
         <v>1</v>
@@ -1637,20 +1649,20 @@
       <c r="J13" s="7">
         <v>0</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="16">
+        <v>0.50117210867155004</v>
+      </c>
+      <c r="L13" s="7">
+        <v>1</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7">
         <v>0.8</v>
       </c>
-      <c r="L13" s="7">
-        <v>1</v>
-      </c>
-      <c r="M13" s="7">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O13" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P13" s="7">
         <v>20</v>
@@ -1658,8 +1670,8 @@
       <c r="Q13" s="7">
         <v>1</v>
       </c>
-      <c r="R13" s="7">
-        <v>0.7</v>
+      <c r="R13" s="14">
+        <v>0.50117210867155004</v>
       </c>
       <c r="S13" s="7">
         <v>2</v>
@@ -1693,8 +1705,8 @@
       <c r="F14" s="8">
         <v>0.5</v>
       </c>
-      <c r="G14" s="7">
-        <v>600</v>
+      <c r="G14" s="15">
+        <v>3500</v>
       </c>
       <c r="H14" s="11">
         <v>0</v>
@@ -1705,20 +1717,20 @@
       <c r="J14" s="7">
         <v>0</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="16">
+        <v>1.4128571428571426</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
         <v>0.8</v>
       </c>
-      <c r="L14" s="7">
-        <v>1</v>
-      </c>
-      <c r="M14" s="7">
-        <v>1</v>
-      </c>
-      <c r="N14" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O14" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P14" s="7">
         <v>20</v>
@@ -1726,8 +1738,8 @@
       <c r="Q14" s="7">
         <v>1</v>
       </c>
-      <c r="R14" s="7">
-        <v>0.7</v>
+      <c r="R14" s="14">
+        <v>4.1208333333333327</v>
       </c>
       <c r="S14" s="7">
         <v>2</v>
@@ -1761,8 +1773,8 @@
       <c r="F15" s="8">
         <v>0.5</v>
       </c>
-      <c r="G15" s="7">
-        <v>2500</v>
+      <c r="G15" s="15">
+        <v>3500</v>
       </c>
       <c r="H15" s="12">
         <v>1</v>
@@ -1773,20 +1785,20 @@
       <c r="J15" s="7">
         <v>0</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="16">
+        <v>2.4700625355954968</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
+        <v>1</v>
+      </c>
+      <c r="N15" s="7">
         <v>0.8</v>
       </c>
-      <c r="L15" s="7">
-        <v>1</v>
-      </c>
-      <c r="M15" s="7">
-        <v>1</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0.9</v>
-      </c>
       <c r="O15" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="P15" s="7">
         <v>20</v>
@@ -1794,8 +1806,8 @@
       <c r="Q15" s="7">
         <v>1</v>
       </c>
-      <c r="R15" s="7">
-        <v>0.7</v>
+      <c r="R15" s="14">
+        <v>2.4700625355954968</v>
       </c>
       <c r="S15" s="7">
         <v>2</v>
@@ -1817,33 +1829,38 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1) updated libs with latest banshee changes, 2) created lib for HW_IO_Interface, 3) added a fault lib, 4) added the DMS seq lib
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-1065" yWindow="-330" windowWidth="28830" windowHeight="5100"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">relays!$A$1:$V$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -199,9 +199,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,6 +214,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -529,7 +529,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,7 +564,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -887,9 +887,9 @@
         <v>0.5</v>
       </c>
       <c r="F2" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="15">
+        <v>13</v>
+      </c>
+      <c r="G2" s="14">
         <v>1200</v>
       </c>
       <c r="H2" s="10">
@@ -901,7 +901,7 @@
       <c r="J2" s="7">
         <v>0</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="15">
         <v>0.60140653040586012</v>
       </c>
       <c r="L2" s="7">
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O2" s="7">
         <v>1.2</v>
@@ -920,22 +920,22 @@
         <v>20</v>
       </c>
       <c r="Q2" s="7">
-        <v>1</v>
-      </c>
-      <c r="R2" s="14">
+        <v>0</v>
+      </c>
+      <c r="R2" s="15">
         <v>0.60140653040586012</v>
       </c>
       <c r="S2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U2" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V2" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -946,18 +946,18 @@
         <v>13800</v>
       </c>
       <c r="C3" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" s="8">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F3" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="15">
+        <v>13</v>
+      </c>
+      <c r="G3" s="14">
         <v>1200</v>
       </c>
       <c r="H3" s="10">
@@ -969,8 +969,8 @@
       <c r="J3" s="7">
         <v>0</v>
       </c>
-      <c r="K3" s="16">
-        <v>2.9124092514083011</v>
+      <c r="K3" s="15">
+        <v>1.4701175847416352</v>
       </c>
       <c r="L3" s="7">
         <v>1</v>
@@ -979,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O3" s="7">
         <v>1.2</v>
@@ -988,22 +988,22 @@
         <v>20</v>
       </c>
       <c r="Q3" s="7">
-        <v>1</v>
-      </c>
-      <c r="R3" s="14">
-        <v>2.9124092514083011</v>
+        <v>0</v>
+      </c>
+      <c r="R3" s="15">
+        <v>1.4701175847416352</v>
       </c>
       <c r="S3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U3" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V3" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1023,9 +1023,9 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="15">
+        <v>13</v>
+      </c>
+      <c r="G4" s="14">
         <v>1200</v>
       </c>
       <c r="H4" s="10">
@@ -1037,7 +1037,7 @@
       <c r="J4" s="7">
         <v>0</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="15">
         <v>1.3030474825460301</v>
       </c>
       <c r="L4" s="7">
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O4" s="7">
         <v>1.2</v>
@@ -1056,22 +1056,22 @@
         <v>20</v>
       </c>
       <c r="Q4" s="7">
-        <v>1</v>
-      </c>
-      <c r="R4" s="14">
+        <v>0</v>
+      </c>
+      <c r="R4" s="15">
         <v>1.3030474825460301</v>
       </c>
       <c r="S4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U4" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V4" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1091,9 +1091,9 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="15">
+        <v>13</v>
+      </c>
+      <c r="G5" s="14">
         <v>1200</v>
       </c>
       <c r="H5" s="10">
@@ -1105,7 +1105,7 @@
       <c r="J5" s="7">
         <v>0</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="15">
         <v>0.10023442173431002</v>
       </c>
       <c r="L5" s="7">
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O5" s="7">
         <v>1.2</v>
@@ -1124,22 +1124,22 @@
         <v>20</v>
       </c>
       <c r="Q5" s="7">
-        <v>1</v>
-      </c>
-      <c r="R5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="15">
         <v>0.10023442173431002</v>
       </c>
       <c r="S5" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T5" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U5" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V5" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1159,9 +1159,9 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="15">
+        <v>13</v>
+      </c>
+      <c r="G6" s="14">
         <v>1200</v>
       </c>
       <c r="H6" s="10">
@@ -1173,7 +1173,7 @@
       <c r="J6" s="7">
         <v>0</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="15">
         <v>0.50117210867155004</v>
       </c>
       <c r="L6" s="7">
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O6" s="7">
         <v>1.2</v>
@@ -1192,22 +1192,22 @@
         <v>20</v>
       </c>
       <c r="Q6" s="7">
-        <v>1</v>
-      </c>
-      <c r="R6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="15">
         <v>0.50117210867155004</v>
       </c>
       <c r="S6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U6" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V6" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1227,9 +1227,9 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="15">
+        <v>13</v>
+      </c>
+      <c r="G7" s="14">
         <v>1200</v>
       </c>
       <c r="H7" s="10">
@@ -1241,7 +1241,7 @@
       <c r="J7" s="7">
         <v>0</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="15">
         <v>0.75175816300732523</v>
       </c>
       <c r="L7" s="7">
@@ -1251,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O7" s="7">
         <v>1.2</v>
@@ -1260,22 +1260,22 @@
         <v>20</v>
       </c>
       <c r="Q7" s="7">
-        <v>1</v>
-      </c>
-      <c r="R7" s="14">
+        <v>0</v>
+      </c>
+      <c r="R7" s="15">
         <v>0.75175816300732523</v>
       </c>
       <c r="S7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U7" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V7" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1295,9 +1295,9 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="15">
+        <v>13</v>
+      </c>
+      <c r="G8" s="14">
         <v>1200</v>
       </c>
       <c r="H8" s="10">
@@ -1309,7 +1309,7 @@
       <c r="J8" s="7">
         <v>0</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="15">
         <v>0.10023442173431002</v>
       </c>
       <c r="L8" s="7">
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O8" s="7">
         <v>1.2</v>
@@ -1328,22 +1328,22 @@
         <v>20</v>
       </c>
       <c r="Q8" s="7">
-        <v>1</v>
-      </c>
-      <c r="R8" s="14">
+        <v>0</v>
+      </c>
+      <c r="R8" s="15">
         <v>0.10023442173431002</v>
       </c>
       <c r="S8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T8" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U8" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V8" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1363,9 +1363,9 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="15">
+        <v>13</v>
+      </c>
+      <c r="G9" s="14">
         <v>1200</v>
       </c>
       <c r="H9" s="11">
@@ -1377,7 +1377,7 @@
       <c r="J9" s="7">
         <v>0</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="15">
         <v>2.0604166666666663</v>
       </c>
       <c r="L9" s="7">
@@ -1387,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O9" s="7">
         <v>1.2</v>
@@ -1396,22 +1396,22 @@
         <v>20</v>
       </c>
       <c r="Q9" s="7">
-        <v>1</v>
-      </c>
-      <c r="R9" s="14">
+        <v>0</v>
+      </c>
+      <c r="R9" s="15">
         <v>2.0604166666666663</v>
       </c>
       <c r="S9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T9" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U9" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V9" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1431,9 +1431,9 @@
         <v>0.5</v>
       </c>
       <c r="F10" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="15">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14">
         <v>3500</v>
       </c>
       <c r="H10" s="11">
@@ -1445,7 +1445,7 @@
       <c r="J10" s="7">
         <v>0</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="15">
         <v>1.4128571428571426</v>
       </c>
       <c r="L10" s="7">
@@ -1455,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O10" s="7">
         <v>1.2</v>
@@ -1464,22 +1464,22 @@
         <v>20</v>
       </c>
       <c r="Q10" s="7">
-        <v>1</v>
-      </c>
-      <c r="R10" s="14">
-        <v>4.1208333333333327</v>
+        <v>0</v>
+      </c>
+      <c r="R10" s="15">
+        <v>1.4128571428571426</v>
       </c>
       <c r="S10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T10" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U10" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V10" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1499,9 +1499,9 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="15">
+        <v>13</v>
+      </c>
+      <c r="G11" s="14">
         <v>1200</v>
       </c>
       <c r="H11" s="10">
@@ -1513,7 +1513,7 @@
       <c r="J11" s="7">
         <v>0</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="15">
         <v>1.3300336730129598</v>
       </c>
       <c r="L11" s="7">
@@ -1523,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O11" s="7">
         <v>1.2</v>
@@ -1532,22 +1532,22 @@
         <v>20</v>
       </c>
       <c r="Q11" s="7">
-        <v>1</v>
-      </c>
-      <c r="R11" s="14">
+        <v>0</v>
+      </c>
+      <c r="R11" s="15">
         <v>1.3300336730129598</v>
       </c>
       <c r="S11" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U11" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V11" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1567,9 +1567,9 @@
         <v>0.5</v>
       </c>
       <c r="F12" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G12" s="15">
+        <v>13</v>
+      </c>
+      <c r="G12" s="14">
         <v>3500</v>
       </c>
       <c r="H12" s="11">
@@ -1581,7 +1581,7 @@
       <c r="J12" s="7">
         <v>0</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="15">
         <v>1.4128571428571426</v>
       </c>
       <c r="L12" s="7">
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O12" s="7">
         <v>1.2</v>
@@ -1600,22 +1600,22 @@
         <v>20</v>
       </c>
       <c r="Q12" s="7">
-        <v>1</v>
-      </c>
-      <c r="R12" s="14">
-        <v>4.1208333333333327</v>
+        <v>0</v>
+      </c>
+      <c r="R12" s="15">
+        <v>1.4128571428571426</v>
       </c>
       <c r="S12" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T12" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U12" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V12" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1635,9 +1635,9 @@
         <v>0.5</v>
       </c>
       <c r="F13" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="15">
+        <v>13</v>
+      </c>
+      <c r="G13" s="14">
         <v>1200</v>
       </c>
       <c r="H13" s="10">
@@ -1649,7 +1649,7 @@
       <c r="J13" s="7">
         <v>0</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="15">
         <v>0.50117210867155004</v>
       </c>
       <c r="L13" s="7">
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O13" s="7">
         <v>1.2</v>
@@ -1668,22 +1668,22 @@
         <v>20</v>
       </c>
       <c r="Q13" s="7">
-        <v>1</v>
-      </c>
-      <c r="R13" s="14">
+        <v>0</v>
+      </c>
+      <c r="R13" s="15">
         <v>0.50117210867155004</v>
       </c>
       <c r="S13" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T13" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U13" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V13" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1703,9 +1703,9 @@
         <v>0.5</v>
       </c>
       <c r="F14" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="15">
+        <v>13</v>
+      </c>
+      <c r="G14" s="14">
         <v>3500</v>
       </c>
       <c r="H14" s="11">
@@ -1717,7 +1717,7 @@
       <c r="J14" s="7">
         <v>0</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="15">
         <v>1.4128571428571426</v>
       </c>
       <c r="L14" s="7">
@@ -1727,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O14" s="7">
         <v>1.2</v>
@@ -1736,22 +1736,22 @@
         <v>20</v>
       </c>
       <c r="Q14" s="7">
-        <v>1</v>
-      </c>
-      <c r="R14" s="14">
-        <v>4.1208333333333327</v>
+        <v>0</v>
+      </c>
+      <c r="R14" s="15">
+        <v>1.4128571428571426</v>
       </c>
       <c r="S14" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T14" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U14" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V14" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1771,9 +1771,9 @@
         <v>0.5</v>
       </c>
       <c r="F15" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="14">
         <v>3500</v>
       </c>
       <c r="H15" s="12">
@@ -1785,7 +1785,7 @@
       <c r="J15" s="7">
         <v>0</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="15">
         <v>2.4700625355954968</v>
       </c>
       <c r="L15" s="7">
@@ -1795,7 +1795,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O15" s="7">
         <v>1.2</v>
@@ -1804,22 +1804,22 @@
         <v>20</v>
       </c>
       <c r="Q15" s="7">
-        <v>1</v>
-      </c>
-      <c r="R15" s="14">
+        <v>0</v>
+      </c>
+      <c r="R15" s="15">
         <v>2.4700625355954968</v>
       </c>
       <c r="S15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T15" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U15" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="V15" s="7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
opened the sync dV for the 480V level relays
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
@@ -776,7 +776,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
         <v>0.5</v>
       </c>
       <c r="F2" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G2" s="14">
         <v>1200</v>
@@ -955,7 +955,7 @@
         <v>0.5</v>
       </c>
       <c r="F3" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G3" s="14">
         <v>1200</v>
@@ -1023,7 +1023,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G4" s="14">
         <v>1200</v>
@@ -1091,7 +1091,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G5" s="14">
         <v>1200</v>
@@ -1159,7 +1159,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G6" s="14">
         <v>1200</v>
@@ -1227,7 +1227,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14">
         <v>1200</v>
@@ -1295,7 +1295,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G8" s="14">
         <v>1200</v>
@@ -1363,7 +1363,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G9" s="14">
         <v>1200</v>
@@ -1422,7 +1422,7 @@
         <v>480</v>
       </c>
       <c r="C10" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D10" s="8">
         <v>12</v>
@@ -1431,7 +1431,7 @@
         <v>0.5</v>
       </c>
       <c r="F10" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G10" s="14">
         <v>3500</v>
@@ -1499,7 +1499,7 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G11" s="14">
         <v>1200</v>
@@ -1567,7 +1567,7 @@
         <v>0.5</v>
       </c>
       <c r="F12" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14">
         <v>3500</v>
@@ -1635,7 +1635,7 @@
         <v>0.5</v>
       </c>
       <c r="F13" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G13" s="14">
         <v>1200</v>
@@ -1694,7 +1694,7 @@
         <v>480</v>
       </c>
       <c r="C14" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8">
         <v>12</v>
@@ -1703,7 +1703,7 @@
         <v>0.5</v>
       </c>
       <c r="F14" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G14" s="14">
         <v>3500</v>
@@ -1762,7 +1762,7 @@
         <v>480</v>
       </c>
       <c r="C15" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8">
         <v>12</v>
@@ -1771,7 +1771,7 @@
         <v>0.5</v>
       </c>
       <c r="F15" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G15" s="14">
         <v>3500</v>

</xml_diff>

<commit_message>
25A element - changed dV from 5% to 10%
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
@@ -776,7 +776,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +878,7 @@
         <v>13800</v>
       </c>
       <c r="C2" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" s="8">
         <v>12</v>
@@ -946,7 +946,7 @@
         <v>13800</v>
       </c>
       <c r="C3" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="8">
         <v>12</v>
@@ -1014,7 +1014,7 @@
         <v>13800</v>
       </c>
       <c r="C4" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8">
         <v>12</v>
@@ -1082,7 +1082,7 @@
         <v>13800</v>
       </c>
       <c r="C5" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5" s="8">
         <v>12</v>
@@ -1150,7 +1150,7 @@
         <v>13800</v>
       </c>
       <c r="C6" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8">
         <v>12</v>
@@ -1218,7 +1218,7 @@
         <v>13800</v>
       </c>
       <c r="C7" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8">
         <v>12</v>
@@ -1286,7 +1286,7 @@
         <v>13800</v>
       </c>
       <c r="C8" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8">
         <v>12</v>
@@ -1354,7 +1354,7 @@
         <v>13800</v>
       </c>
       <c r="C9" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8">
         <v>12</v>
@@ -1490,7 +1490,7 @@
         <v>4160</v>
       </c>
       <c r="C11" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8">
         <v>12</v>
@@ -1558,7 +1558,7 @@
         <v>4160</v>
       </c>
       <c r="C12" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D12" s="8">
         <v>12</v>
@@ -1626,7 +1626,7 @@
         <v>13800</v>
       </c>
       <c r="C13" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8">
         <v>12</v>

</xml_diff>

<commit_message>
Updated F1-F3 relay settings with 81 functions
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F1_relay_banshee.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1065" yWindow="-330" windowWidth="28830" windowHeight="5100"/>
+    <workbookView xWindow="-1068" yWindow="-336" windowWidth="23256" windowHeight="5100"/>
   </bookViews>
   <sheets>
     <sheet name="relays" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">relays!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">relays!$A$1:$AC$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>VRMSLL</t>
   </si>
@@ -66,11 +66,34 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>81U Trip Pickup [Hz]</t>
+  </si>
+  <si>
+    <t>81U Trip Delay [Sec]</t>
+  </si>
+  <si>
+    <t>81O Trip Pickup [Hz]</t>
+  </si>
+  <si>
+    <t>81O Trip Delay [Sec]</t>
+  </si>
+  <si>
+    <t>81RFRP
+[Hz/Sec]</t>
+  </si>
+  <si>
+    <t>81RFDFP
+[Hz]</t>
+  </si>
+  <si>
+    <t>81RF Trip Delay [Sec]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -204,6 +227,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,6 +509,44 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>891540</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>876582</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>53563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886700" y="3467100"/>
+          <a:ext cx="3254022" cy="2568163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -529,7 +593,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,7 +628,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -773,36 +837,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="14" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
-    <col min="5" max="6" width="17.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="7" customWidth="1"/>
+    <col min="5" max="6" width="17.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="7" customWidth="1"/>
     <col min="8" max="8" width="18" style="7" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="7" customWidth="1"/>
     <col min="11" max="11" width="17" style="7" customWidth="1"/>
-    <col min="12" max="15" width="12.140625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="7" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" style="7" customWidth="1"/>
-    <col min="19" max="20" width="12.140625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" style="7" customWidth="1"/>
-    <col min="23" max="24" width="17.28515625" style="7" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="7"/>
+    <col min="12" max="15" width="12.109375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13" style="7" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="7" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" style="7" customWidth="1"/>
+    <col min="20" max="21" width="9.109375" style="7"/>
+    <col min="22" max="22" width="11.109375" style="7" customWidth="1"/>
+    <col min="23" max="23" width="18.109375" style="7" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" style="7" customWidth="1"/>
+    <col min="25" max="25" width="17.44140625" style="7" customWidth="1"/>
+    <col min="26" max="27" width="12.109375" style="7" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" style="7" customWidth="1"/>
+    <col min="29" max="29" width="11.88671875" style="7" customWidth="1"/>
+    <col min="30" max="30" width="13.44140625" style="7" customWidth="1"/>
+    <col min="31" max="31" width="13" style="7" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" style="7" customWidth="1"/>
+    <col min="33" max="33" width="12.109375" style="7" customWidth="1"/>
+    <col min="34" max="35" width="9.109375" style="7"/>
+    <col min="36" max="36" width="11.109375" style="7" customWidth="1"/>
+    <col min="37" max="38" width="17.33203125" style="7" customWidth="1"/>
+    <col min="39" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -848,29 +924,71 @@
       <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="AD1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -917,28 +1035,70 @@
         <v>1.2</v>
       </c>
       <c r="P2" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="7">
-        <v>0</v>
-      </c>
-      <c r="R2" s="15">
+        <v>2</v>
+      </c>
+      <c r="R2" s="7">
+        <v>66</v>
+      </c>
+      <c r="S2" s="7">
+        <v>2</v>
+      </c>
+      <c r="T2" s="7">
+        <v>2</v>
+      </c>
+      <c r="U2" s="7">
+        <v>57</v>
+      </c>
+      <c r="V2" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W2" s="7">
+        <v>20</v>
+      </c>
+      <c r="X2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="15">
         <v>0.60140653040586012</v>
       </c>
-      <c r="S2" s="7">
-        <v>1</v>
-      </c>
-      <c r="T2" s="7">
-        <v>1</v>
-      </c>
-      <c r="U2" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V2" s="7">
-        <v>1.2</v>
+      <c r="Z2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -985,28 +1145,70 @@
         <v>1.2</v>
       </c>
       <c r="P3" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q3" s="7">
-        <v>0</v>
-      </c>
-      <c r="R3" s="15">
+        <v>2</v>
+      </c>
+      <c r="R3" s="7">
+        <v>66</v>
+      </c>
+      <c r="S3" s="7">
+        <v>2</v>
+      </c>
+      <c r="T3" s="7">
+        <v>2</v>
+      </c>
+      <c r="U3" s="7">
+        <v>57</v>
+      </c>
+      <c r="V3" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W3" s="7">
+        <v>20</v>
+      </c>
+      <c r="X3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="15">
         <v>1.4701175847416352</v>
       </c>
-      <c r="S3" s="7">
-        <v>1</v>
-      </c>
-      <c r="T3" s="7">
-        <v>1</v>
-      </c>
-      <c r="U3" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V3" s="7">
-        <v>1.2</v>
+      <c r="Z3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD3" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ3" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1053,28 +1255,70 @@
         <v>1.2</v>
       </c>
       <c r="P4" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="7">
-        <v>0</v>
-      </c>
-      <c r="R4" s="15">
+        <v>2</v>
+      </c>
+      <c r="R4" s="7">
+        <v>66</v>
+      </c>
+      <c r="S4" s="7">
+        <v>2</v>
+      </c>
+      <c r="T4" s="7">
+        <v>2</v>
+      </c>
+      <c r="U4" s="7">
+        <v>57</v>
+      </c>
+      <c r="V4" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W4" s="7">
+        <v>20</v>
+      </c>
+      <c r="X4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="15">
         <v>1.3030474825460301</v>
       </c>
-      <c r="S4" s="7">
-        <v>1</v>
-      </c>
-      <c r="T4" s="7">
-        <v>1</v>
-      </c>
-      <c r="U4" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V4" s="7">
-        <v>1.2</v>
+      <c r="Z4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC4" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD4" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG4" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ4" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1121,28 +1365,70 @@
         <v>1.2</v>
       </c>
       <c r="P5" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="7">
-        <v>0</v>
-      </c>
-      <c r="R5" s="15">
+        <v>2</v>
+      </c>
+      <c r="R5" s="7">
+        <v>66</v>
+      </c>
+      <c r="S5" s="7">
+        <v>2</v>
+      </c>
+      <c r="T5" s="7">
+        <v>2</v>
+      </c>
+      <c r="U5" s="7">
+        <v>57</v>
+      </c>
+      <c r="V5" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W5" s="7">
+        <v>20</v>
+      </c>
+      <c r="X5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="15">
         <v>0.10023442173431002</v>
       </c>
-      <c r="S5" s="7">
-        <v>1</v>
-      </c>
-      <c r="T5" s="7">
-        <v>1</v>
-      </c>
-      <c r="U5" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V5" s="7">
-        <v>1.2</v>
+      <c r="Z5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD5" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE5" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG5" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1189,28 +1475,70 @@
         <v>1.2</v>
       </c>
       <c r="P6" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="7">
-        <v>0</v>
-      </c>
-      <c r="R6" s="15">
+        <v>2</v>
+      </c>
+      <c r="R6" s="7">
+        <v>66</v>
+      </c>
+      <c r="S6" s="7">
+        <v>2</v>
+      </c>
+      <c r="T6" s="7">
+        <v>2</v>
+      </c>
+      <c r="U6" s="7">
+        <v>57</v>
+      </c>
+      <c r="V6" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W6" s="7">
+        <v>20</v>
+      </c>
+      <c r="X6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="15">
         <v>0.50117210867155004</v>
       </c>
-      <c r="S6" s="7">
-        <v>1</v>
-      </c>
-      <c r="T6" s="7">
-        <v>1</v>
-      </c>
-      <c r="U6" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V6" s="7">
-        <v>1.2</v>
+      <c r="Z6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD6" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE6" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG6" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ6" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1257,28 +1585,70 @@
         <v>1.2</v>
       </c>
       <c r="P7" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q7" s="7">
-        <v>0</v>
-      </c>
-      <c r="R7" s="15">
+        <v>2</v>
+      </c>
+      <c r="R7" s="7">
+        <v>66</v>
+      </c>
+      <c r="S7" s="7">
+        <v>2</v>
+      </c>
+      <c r="T7" s="7">
+        <v>2</v>
+      </c>
+      <c r="U7" s="7">
+        <v>57</v>
+      </c>
+      <c r="V7" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W7" s="7">
+        <v>20</v>
+      </c>
+      <c r="X7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="15">
         <v>0.75175816300732523</v>
       </c>
-      <c r="S7" s="7">
-        <v>1</v>
-      </c>
-      <c r="T7" s="7">
-        <v>1</v>
-      </c>
-      <c r="U7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V7" s="7">
-        <v>1.2</v>
+      <c r="Z7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC7" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD7" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE7" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG7" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ7" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1325,28 +1695,70 @@
         <v>1.2</v>
       </c>
       <c r="P8" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q8" s="7">
-        <v>0</v>
-      </c>
-      <c r="R8" s="15">
+        <v>2</v>
+      </c>
+      <c r="R8" s="7">
+        <v>66</v>
+      </c>
+      <c r="S8" s="7">
+        <v>2</v>
+      </c>
+      <c r="T8" s="7">
+        <v>2</v>
+      </c>
+      <c r="U8" s="7">
+        <v>57</v>
+      </c>
+      <c r="V8" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W8" s="7">
+        <v>20</v>
+      </c>
+      <c r="X8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="15">
         <v>0.10023442173431002</v>
       </c>
-      <c r="S8" s="7">
-        <v>1</v>
-      </c>
-      <c r="T8" s="7">
-        <v>1</v>
-      </c>
-      <c r="U8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V8" s="7">
-        <v>1.2</v>
+      <c r="Z8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG8" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ8" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1393,28 +1805,70 @@
         <v>1.2</v>
       </c>
       <c r="P9" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q9" s="7">
-        <v>0</v>
-      </c>
-      <c r="R9" s="15">
+        <v>2</v>
+      </c>
+      <c r="R9" s="7">
+        <v>66</v>
+      </c>
+      <c r="S9" s="7">
+        <v>2</v>
+      </c>
+      <c r="T9" s="7">
+        <v>2</v>
+      </c>
+      <c r="U9" s="7">
+        <v>57</v>
+      </c>
+      <c r="V9" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W9" s="7">
+        <v>20</v>
+      </c>
+      <c r="X9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="15">
         <v>2.0604166666666663</v>
       </c>
-      <c r="S9" s="7">
-        <v>1</v>
-      </c>
-      <c r="T9" s="7">
-        <v>1</v>
-      </c>
-      <c r="U9" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V9" s="7">
-        <v>1.2</v>
+      <c r="Z9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE9" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG9" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH9" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ9" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1461,28 +1915,70 @@
         <v>1.2</v>
       </c>
       <c r="P10" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q10" s="7">
-        <v>0</v>
-      </c>
-      <c r="R10" s="15">
+        <v>2</v>
+      </c>
+      <c r="R10" s="7">
+        <v>66</v>
+      </c>
+      <c r="S10" s="7">
+        <v>2</v>
+      </c>
+      <c r="T10" s="7">
+        <v>2</v>
+      </c>
+      <c r="U10" s="7">
+        <v>57</v>
+      </c>
+      <c r="V10" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W10" s="7">
+        <v>20</v>
+      </c>
+      <c r="X10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="15">
         <v>1.4128571428571426</v>
       </c>
-      <c r="S10" s="7">
-        <v>1</v>
-      </c>
-      <c r="T10" s="7">
-        <v>1</v>
-      </c>
-      <c r="U10" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V10" s="7">
-        <v>1.2</v>
+      <c r="Z10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ10" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1529,28 +2025,70 @@
         <v>1.2</v>
       </c>
       <c r="P11" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q11" s="7">
-        <v>0</v>
-      </c>
-      <c r="R11" s="15">
+        <v>2</v>
+      </c>
+      <c r="R11" s="7">
+        <v>66</v>
+      </c>
+      <c r="S11" s="7">
+        <v>2</v>
+      </c>
+      <c r="T11" s="7">
+        <v>2</v>
+      </c>
+      <c r="U11" s="7">
+        <v>57</v>
+      </c>
+      <c r="V11" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W11" s="7">
+        <v>20</v>
+      </c>
+      <c r="X11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="15">
         <v>1.3300336730129598</v>
       </c>
-      <c r="S11" s="7">
-        <v>1</v>
-      </c>
-      <c r="T11" s="7">
-        <v>1</v>
-      </c>
-      <c r="U11" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V11" s="7">
-        <v>1.2</v>
+      <c r="Z11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD11" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE11" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG11" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ11" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1597,28 +2135,70 @@
         <v>1.2</v>
       </c>
       <c r="P12" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q12" s="7">
-        <v>0</v>
-      </c>
-      <c r="R12" s="15">
+        <v>2</v>
+      </c>
+      <c r="R12" s="7">
+        <v>66</v>
+      </c>
+      <c r="S12" s="7">
+        <v>2</v>
+      </c>
+      <c r="T12" s="7">
+        <v>2</v>
+      </c>
+      <c r="U12" s="7">
+        <v>57</v>
+      </c>
+      <c r="V12" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W12" s="7">
+        <v>20</v>
+      </c>
+      <c r="X12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="15">
         <v>1.4128571428571426</v>
       </c>
-      <c r="S12" s="7">
-        <v>1</v>
-      </c>
-      <c r="T12" s="7">
-        <v>1</v>
-      </c>
-      <c r="U12" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V12" s="7">
-        <v>1.2</v>
+      <c r="Z12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC12" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD12" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE12" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG12" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH12" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ12" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1665,28 +2245,70 @@
         <v>1.2</v>
       </c>
       <c r="P13" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q13" s="7">
-        <v>0</v>
-      </c>
-      <c r="R13" s="15">
+        <v>2</v>
+      </c>
+      <c r="R13" s="7">
+        <v>66</v>
+      </c>
+      <c r="S13" s="7">
+        <v>2</v>
+      </c>
+      <c r="T13" s="7">
+        <v>2</v>
+      </c>
+      <c r="U13" s="7">
+        <v>57</v>
+      </c>
+      <c r="V13" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W13" s="7">
+        <v>20</v>
+      </c>
+      <c r="X13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="15">
         <v>0.50117210867155004</v>
       </c>
-      <c r="S13" s="7">
-        <v>1</v>
-      </c>
-      <c r="T13" s="7">
-        <v>1</v>
-      </c>
-      <c r="U13" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V13" s="7">
-        <v>1.2</v>
+      <c r="Z13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD13" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE13" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG13" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ13" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1733,28 +2355,70 @@
         <v>1.2</v>
       </c>
       <c r="P14" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q14" s="7">
-        <v>0</v>
-      </c>
-      <c r="R14" s="15">
+        <v>2</v>
+      </c>
+      <c r="R14" s="7">
+        <v>66</v>
+      </c>
+      <c r="S14" s="7">
+        <v>2</v>
+      </c>
+      <c r="T14" s="7">
+        <v>2</v>
+      </c>
+      <c r="U14" s="7">
+        <v>57</v>
+      </c>
+      <c r="V14" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W14" s="7">
+        <v>20</v>
+      </c>
+      <c r="X14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="15">
         <v>1.4128571428571426</v>
       </c>
-      <c r="S14" s="7">
-        <v>1</v>
-      </c>
-      <c r="T14" s="7">
-        <v>1</v>
-      </c>
-      <c r="U14" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V14" s="7">
-        <v>1.2</v>
+      <c r="Z14" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD14" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF14" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG14" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH14" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI14" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ14" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -1801,63 +2465,105 @@
         <v>1.2</v>
       </c>
       <c r="P15" s="7">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="7">
-        <v>0</v>
-      </c>
-      <c r="R15" s="15">
+        <v>2</v>
+      </c>
+      <c r="R15" s="7">
+        <v>66</v>
+      </c>
+      <c r="S15" s="7">
+        <v>2</v>
+      </c>
+      <c r="T15" s="7">
+        <v>2</v>
+      </c>
+      <c r="U15" s="7">
+        <v>57</v>
+      </c>
+      <c r="V15" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="W15" s="7">
+        <v>20</v>
+      </c>
+      <c r="X15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="15">
         <v>2.4700625355954968</v>
       </c>
-      <c r="S15" s="7">
-        <v>1</v>
-      </c>
-      <c r="T15" s="7">
-        <v>1</v>
-      </c>
-      <c r="U15" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="V15" s="7">
-        <v>1.2</v>
+      <c r="Z15" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AD15" s="7">
+        <v>54</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="7">
+        <v>66</v>
+      </c>
+      <c r="AG15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI15" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ15" s="7">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K21" s="7" t="s">
         <v>15</v>
       </c>

</xml_diff>